<commit_message>
Họp Demo sửa lỗi
</commit_message>
<xml_diff>
--- a/PhieuDanhGia-PTUDW-DACK-Ads-Nhom7.xlsx
+++ b/PhieuDanhGia-PTUDW-DACK-Ads-Nhom7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Ads-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0AAE55-8830-418E-8609-7876E5380CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750BE8AF-9C3F-483B-AA9F-3F0C5F0993E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,16 +283,16 @@
     <t>Khuyến khích sử dụng template &amp; các thư viện css, jQuery, …</t>
   </si>
   <si>
-    <t>Đỗ Thế Nghĩa</t>
+    <t>Đỗ Thế Nghĩa - 21127367</t>
   </si>
   <si>
-    <t>Nguyễn Anh Khoa</t>
+    <t>Nguyễn Anh Khoa - 21127517</t>
   </si>
   <si>
-    <t>Nguyễn Lâm Hải</t>
+    <t>Nguyễn Lâm Hải - 21127604</t>
   </si>
   <si>
-    <t>Nguyễn Phú Minh Bảo</t>
+    <t>Nguyễn Phú Minh Bảo - 21127013</t>
   </si>
 </sst>
 </file>
@@ -631,6 +631,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -642,12 +648,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -879,12 +879,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:26" ht="20.25" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -921,14 +921,18 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A3" s="48">
+      <c r="A3" s="43">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
+      <c r="C3" s="6">
+        <v>10</v>
+      </c>
+      <c r="D3" s="7">
+        <v>10</v>
+      </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -953,14 +957,18 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A4" s="49">
+      <c r="A4" s="44">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="C4" s="9">
+        <v>10</v>
+      </c>
+      <c r="D4" s="10">
+        <v>10</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -985,14 +993,18 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A5" s="49">
+      <c r="A5" s="44">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="C5" s="9">
+        <v>10</v>
+      </c>
+      <c r="D5" s="10">
+        <v>10</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1017,14 +1029,18 @@
       <c r="Z5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A6" s="49">
+      <c r="A6" s="44">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="C6" s="9">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10">
+        <v>10</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -1049,7 +1065,7 @@
       <c r="Z6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A7" s="49">
+      <c r="A7" s="44">
         <v>5</v>
       </c>
       <c r="B7" s="8"/>
@@ -1107,12 +1123,12 @@
       <c r="Z8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1137,12 +1153,12 @@
       <c r="Z9" s="4"/>
     </row>
     <row r="10" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1291,10 +1307,10 @@
       <c r="Z14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="30" customHeight="1">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="47"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="23">
         <v>-0.25</v>
       </c>
@@ -1424,7 +1440,9 @@
       <c r="C19" s="20">
         <v>-0.5</v>
       </c>
-      <c r="D19" s="21"/>
+      <c r="D19" s="21">
+        <v>0</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -2228,7 +2246,9 @@
       <c r="C43" s="20">
         <v>-1</v>
       </c>
-      <c r="D43" s="21"/>
+      <c r="D43" s="21">
+        <v>0</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2464,7 +2484,9 @@
       <c r="C50" s="20">
         <v>-1</v>
       </c>
-      <c r="D50" s="21"/>
+      <c r="D50" s="21">
+        <v>0</v>
+      </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -2496,7 +2518,9 @@
       <c r="C51" s="20">
         <v>-0.5</v>
       </c>
-      <c r="D51" s="21"/>
+      <c r="D51" s="21">
+        <v>0</v>
+      </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -2528,7 +2552,9 @@
       <c r="C52" s="13">
         <v>-0.5</v>
       </c>
-      <c r="D52" s="14"/>
+      <c r="D52" s="14">
+        <v>0</v>
+      </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -2618,7 +2644,9 @@
       <c r="C55" s="29">
         <v>-0.5</v>
       </c>
-      <c r="D55" s="24"/>
+      <c r="D55" s="24">
+        <v>0</v>
+      </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -2718,7 +2746,9 @@
       <c r="C58" s="29">
         <v>-0.5</v>
       </c>
-      <c r="D58" s="21"/>
+      <c r="D58" s="21">
+        <v>0</v>
+      </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -2784,7 +2814,9 @@
       <c r="C60" s="29">
         <v>-0.5</v>
       </c>
-      <c r="D60" s="21"/>
+      <c r="D60" s="21">
+        <v>0</v>
+      </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -2816,7 +2848,9 @@
       <c r="C61" s="29">
         <v>-0.5</v>
       </c>
-      <c r="D61" s="21"/>
+      <c r="D61" s="21">
+        <v>0</v>
+      </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -2848,7 +2882,9 @@
       <c r="C62" s="29">
         <v>-0.5</v>
       </c>
-      <c r="D62" s="21"/>
+      <c r="D62" s="21">
+        <v>0</v>
+      </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -2914,7 +2950,9 @@
       <c r="C64" s="29">
         <v>-0.5</v>
       </c>
-      <c r="D64" s="21"/>
+      <c r="D64" s="21">
+        <v>0</v>
+      </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>

</xml_diff>